<commit_message>
removed some minor bugs and reformattedthe output.
</commit_message>
<xml_diff>
--- a/truth.xlsx
+++ b/truth.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="truth" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="32">
   <si>
     <t>Present State</t>
   </si>
@@ -80,6 +80,36 @@
   </si>
   <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>"0000"</t>
+  </si>
+  <si>
+    <t>"1000"</t>
+  </si>
+  <si>
+    <t>"1001"</t>
+  </si>
+  <si>
+    <t>"1100"</t>
+  </si>
+  <si>
+    <t>"1010"</t>
+  </si>
+  <si>
+    <t>"1101"</t>
+  </si>
+  <si>
+    <t>"1011"</t>
+  </si>
+  <si>
+    <t>"1110"</t>
+  </si>
+  <si>
+    <t>"1111"</t>
   </si>
 </sst>
 </file>
@@ -156,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -194,6 +224,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -202,7 +254,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,6 +272,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -530,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H62"/>
+  <dimension ref="B1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,24 +605,28 @@
     <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="22.5" x14ac:dyDescent="0.3">
       <c r="B1" s="6"/>
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="I1" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="22.5" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
@@ -577,8 +642,9 @@
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>0</v>
       </c>
@@ -598,8 +664,11 @@
       <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -619,8 +688,11 @@
       <c r="H4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -640,8 +712,11 @@
       <c r="H5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -661,8 +736,11 @@
       <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -682,8 +760,11 @@
       <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -703,8 +784,11 @@
       <c r="H8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -724,8 +808,11 @@
       <c r="H9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>7</v>
       </c>
@@ -745,8 +832,11 @@
       <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>8</v>
       </c>
@@ -766,8 +856,11 @@
       <c r="H11" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>9</v>
       </c>
@@ -787,8 +880,11 @@
       <c r="H12" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>10</v>
       </c>
@@ -808,8 +904,11 @@
       <c r="H13" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>11</v>
       </c>
@@ -829,8 +928,11 @@
       <c r="H14" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>12</v>
       </c>
@@ -850,8 +952,11 @@
       <c r="H15" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>13</v>
       </c>
@@ -871,8 +976,11 @@
       <c r="H16" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>14</v>
       </c>
@@ -892,8 +1000,11 @@
       <c r="H17" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>15</v>
       </c>
@@ -913,8 +1024,11 @@
       <c r="H18" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>16</v>
       </c>
@@ -934,8 +1048,11 @@
       <c r="H19" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>17</v>
       </c>
@@ -955,8 +1072,11 @@
       <c r="H20" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>18</v>
       </c>
@@ -976,8 +1096,11 @@
       <c r="H21" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>19</v>
       </c>
@@ -997,8 +1120,11 @@
       <c r="H22" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>20</v>
       </c>
@@ -1018,8 +1144,11 @@
       <c r="H23" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>21</v>
       </c>
@@ -1039,8 +1168,11 @@
       <c r="H24" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>22</v>
       </c>
@@ -1060,8 +1192,11 @@
       <c r="H25" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>23</v>
       </c>
@@ -1081,8 +1216,11 @@
       <c r="H26" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>24</v>
       </c>
@@ -1102,8 +1240,11 @@
       <c r="H27" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>25</v>
       </c>
@@ -1123,8 +1264,11 @@
       <c r="H28" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>26</v>
       </c>
@@ -1144,8 +1288,11 @@
       <c r="H29" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>27</v>
       </c>
@@ -1165,8 +1312,11 @@
       <c r="H30" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>28</v>
       </c>
@@ -1186,8 +1336,11 @@
       <c r="H31" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>29</v>
       </c>
@@ -1207,8 +1360,11 @@
       <c r="H32" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>30</v>
       </c>
@@ -1228,8 +1384,11 @@
       <c r="H33" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>31</v>
       </c>
@@ -1249,8 +1408,11 @@
       <c r="H34" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>32</v>
       </c>
@@ -1270,8 +1432,11 @@
       <c r="H35" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>33</v>
       </c>
@@ -1291,8 +1456,11 @@
       <c r="H36" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>34</v>
       </c>
@@ -1312,8 +1480,11 @@
       <c r="H37" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>35</v>
       </c>
@@ -1333,8 +1504,11 @@
       <c r="H38" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>36</v>
       </c>
@@ -1354,8 +1528,11 @@
       <c r="H39" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>37</v>
       </c>
@@ -1375,8 +1552,11 @@
       <c r="H40" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>38</v>
       </c>
@@ -1396,8 +1576,11 @@
       <c r="H41" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>39</v>
       </c>
@@ -1417,8 +1600,11 @@
       <c r="H42" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>40</v>
       </c>
@@ -1438,8 +1624,11 @@
       <c r="H43" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>41</v>
       </c>
@@ -1459,8 +1648,11 @@
       <c r="H44" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>42</v>
       </c>
@@ -1480,8 +1672,11 @@
       <c r="H45" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <v>43</v>
       </c>
@@ -1501,8 +1696,11 @@
       <c r="H46" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>44</v>
       </c>
@@ -1522,8 +1720,11 @@
       <c r="H47" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
         <v>45</v>
       </c>
@@ -1543,8 +1744,11 @@
       <c r="H48" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>46</v>
       </c>
@@ -1564,8 +1768,11 @@
       <c r="H49" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="4">
         <v>47</v>
       </c>
@@ -1585,100 +1792,115 @@
       <c r="H50" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="3">
-        <v>48</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="I50" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>52</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0</v>
+      </c>
+      <c r="F51" s="5">
+        <v>0</v>
+      </c>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D51" s="3">
-        <v>1</v>
-      </c>
-      <c r="E51" s="3">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3">
-        <v>0</v>
-      </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="3">
-        <v>49</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="3">
-        <v>1</v>
-      </c>
-      <c r="E52" s="3">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3">
-        <v>1</v>
-      </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="3">
-        <v>50</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="3">
-        <v>1</v>
-      </c>
-      <c r="E53" s="3">
-        <v>1</v>
-      </c>
-      <c r="F53" s="3">
-        <v>0</v>
-      </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="3">
-        <v>51</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="3">
-        <v>1</v>
-      </c>
-      <c r="E54" s="3">
-        <v>1</v>
-      </c>
-      <c r="F54" s="3">
-        <v>1</v>
-      </c>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="4">
+        <v>53</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0</v>
+      </c>
+      <c r="F52" s="5">
+        <v>1</v>
+      </c>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="4">
+        <v>54</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+      <c r="E53" s="5">
+        <v>1</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0</v>
+      </c>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="4">
+        <v>55</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="5">
+        <v>0</v>
+      </c>
+      <c r="E54" s="5">
+        <v>1</v>
+      </c>
+      <c r="F54" s="5">
+        <v>1</v>
+      </c>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="4">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D55" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="5">
         <v>0</v>
@@ -1688,18 +1910,21 @@
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="4">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D56" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="5">
         <v>0</v>
@@ -1709,18 +1934,21 @@
       </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="4">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D57" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" s="5">
         <v>1</v>
@@ -1730,18 +1958,21 @@
       </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="4">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
@@ -1753,89 +1984,8 @@
       <c r="H58" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="4">
-        <v>56</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59" s="5">
-        <v>1</v>
-      </c>
-      <c r="E59" s="5">
-        <v>0</v>
-      </c>
-      <c r="F59" s="5">
-        <v>0</v>
-      </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="4">
-        <v>57</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="5">
-        <v>1</v>
-      </c>
-      <c r="E60" s="5">
-        <v>0</v>
-      </c>
-      <c r="F60" s="5">
-        <v>1</v>
-      </c>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="4">
-        <v>58</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" s="5">
-        <v>1</v>
-      </c>
-      <c r="E61" s="5">
-        <v>1</v>
-      </c>
-      <c r="F61" s="5">
-        <v>0</v>
-      </c>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="4">
-        <v>59</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="5">
-        <v>1</v>
-      </c>
-      <c r="E62" s="5">
-        <v>1</v>
-      </c>
-      <c r="F62" s="5">
-        <v>1</v>
-      </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5" t="s">
-        <v>20</v>
+      <c r="I58" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>